<commit_message>
Generation of Public Bus data with datatypes
Edited yaml file to include datatypes and generated RDF.
</commit_message>
<xml_diff>
--- a/examples/publicBus/InputBus.xlsx
+++ b/examples/publicBus/InputBus.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ednaruckhaus/Documents/GitHub/Mapeathor/examples/publicBus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF39711-DD9E-514E-8ACA-CB56029EA7B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25DEABD-2DA0-F44A-AF42-CBABAB27DC8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4960" yWindow="5040" windowWidth="26300" windowHeight="15600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4960" yWindow="4700" windowWidth="26300" windowHeight="15600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prefixes" sheetId="1" r:id="rId1"/>
-    <sheet name="Subject" sheetId="3" r:id="rId2"/>
-    <sheet name="Source" sheetId="2" r:id="rId3"/>
+    <sheet name="Source" sheetId="2" r:id="rId2"/>
+    <sheet name="Subject" sheetId="3" r:id="rId3"/>
     <sheet name="PredicateObjectMaps" sheetId="4" r:id="rId4"/>
     <sheet name="Functions" sheetId="5" r:id="rId5"/>
   </sheets>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="95">
   <si>
     <t>Prefix</t>
   </si>
@@ -112,18 +112,6 @@
     <t xml:space="preserve">dcterms </t>
   </si>
   <si>
-    <t>http//xmlns.com/foaf/0.1/</t>
-  </si>
-  <si>
-    <t>http//www.w3.org/2001/XMLSchema#</t>
-  </si>
-  <si>
-    <t>http//www.w3.org/2000/01/rdf-schema#</t>
-  </si>
-  <si>
-    <t>http//purl.org/dc/elements/1.1/</t>
-  </si>
-  <si>
     <t xml:space="preserve">esautob </t>
   </si>
   <si>
@@ -323,6 +311,9 @@
   </si>
   <si>
     <t>examples/publicBus/paradas.csv</t>
+  </si>
+  <si>
+    <t>http://xmlns.com/foaf/0.1/</t>
   </si>
 </sst>
 </file>
@@ -709,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -732,32 +723,32 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>27</v>
+      <c r="B2" s="7" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>28</v>
+      <c r="B3" s="7" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>29</v>
+      <c r="B4" s="7" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>30</v>
+      <c r="B5" s="7" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -765,7 +756,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -773,7 +764,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -781,7 +772,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -789,7 +780,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -797,47 +788,47 @@
         <v>26</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -845,87 +836,87 @@
         <v>9</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -935,11 +926,108 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="42.83203125" customWidth="1"/>
+    <col min="2" max="1025" width="10.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -961,132 +1049,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="42.83203125" customWidth="1"/>
-    <col min="2" max="1025" width="10.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1140,197 +1131,197 @@
     </row>
     <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
       </c>
       <c r="G2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
         <v>24</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
         <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C8" t="s">
         <v>24</v>
       </c>
       <c r="G8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C9" t="s">
         <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F9" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E10" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F10" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C11" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C12" t="s">
         <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
         <v>24</v>
       </c>
       <c r="G13" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Examples Traffic and Public Bus
New examples for generating rdf data for validating Traffic and Public Bus vocabularies.
</commit_message>
<xml_diff>
--- a/examples/publicBus/InputBus.xlsx
+++ b/examples/publicBus/InputBus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ednaruckhaus/Documents/GitHub/Mapeathor/examples/publicBus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25DEABD-2DA0-F44A-AF42-CBABAB27DC8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C44811A-B532-0949-A577-410DCFB0BD96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4960" yWindow="4700" windowWidth="26300" windowHeight="15600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8800" yWindow="460" windowWidth="26300" windowHeight="15600" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prefixes" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="94">
   <si>
     <t>Prefix</t>
   </si>
@@ -49,18 +49,12 @@
     <t>dc</t>
   </si>
   <si>
-    <t>dct</t>
-  </si>
-  <si>
     <t>rdf</t>
   </si>
   <si>
     <t>skos</t>
   </si>
   <si>
-    <t>owl</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -109,9 +103,6 @@
     <t>FunctionID</t>
   </si>
   <si>
-    <t xml:space="preserve">dcterms </t>
-  </si>
-  <si>
     <t xml:space="preserve">esautob </t>
   </si>
   <si>
@@ -124,9 +115,6 @@
     <t>idPoint</t>
   </si>
   <si>
-    <t>geosparql:Point</t>
-  </si>
-  <si>
     <t>{stop_code}</t>
   </si>
   <si>
@@ -154,12 +142,6 @@
     <t xml:space="preserve">geosparql </t>
   </si>
   <si>
-    <t xml:space="preserve">rdf </t>
-  </si>
-  <si>
-    <t xml:space="preserve">rdfs </t>
-  </si>
-  <si>
     <t xml:space="preserve">schema </t>
   </si>
   <si>
@@ -268,9 +250,6 @@
     <t>http://www.opengis.net/doc/IS/geosparql/1.0#</t>
   </si>
   <si>
-    <t>http://www.w3.org/2002/07/owl#</t>
-  </si>
-  <si>
     <t>http://www.w3.org/2000/01/rdf-schema#</t>
   </si>
   <si>
@@ -314,6 +293,24 @@
   </si>
   <si>
     <t>http://xmlns.com/foaf/0.1/</t>
+  </si>
+  <si>
+    <t>geo_core</t>
+  </si>
+  <si>
+    <t>sf</t>
+  </si>
+  <si>
+    <t>http://www.opengis.net/ont/sf#</t>
+  </si>
+  <si>
+    <t>https://datos.ign.es/def/geo_core#</t>
+  </si>
+  <si>
+    <t>sf:Point</t>
+  </si>
+  <si>
+    <t>dcterms</t>
   </si>
 </sst>
 </file>
@@ -698,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -724,7 +721,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -732,7 +729,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -740,7 +737,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -748,175 +745,151 @@
         <v>5</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>93</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>45</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>82</v>
+        <v>58</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>83</v>
+        <v>88</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>89</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>48</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>66</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>64</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -930,7 +903,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -941,79 +914,79 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1027,7 +1000,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1038,10 +1011,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1049,35 +1022,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>92</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1090,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1108,220 +1081,220 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F9" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E10" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F10" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G13" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1346,13 +1319,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>